<commit_message>
Upravena verze xlsx souboru
</commit_message>
<xml_diff>
--- a/M365/hromadneVytvoreniZamestnancu/hromadneVytvoreniZamestnancu.xlsx
+++ b/M365/hromadneVytvoreniZamestnancu/hromadneVytvoreniZamestnancu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://examplemblab-my.sharepoint.com/personal/marek_bubenik_mblab_cloud1/Documents/Dokumenty/Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c26969d82fe7094/Dokumenty/Personal/mslab/M365/hromadneVytvoreniZamestnancu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{1D09394C-FB05-44F8-B5A6-149DE08BE8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{382D43E3-5457-4A6D-A5AE-67C0F7906405}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{1D09394C-FB05-44F8-B5A6-149DE08BE8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E08C9292-7466-4117-8CB8-C55869204966}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hromadneVytvoreniZamestnancu" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>version:v1.0</t>
   </si>
@@ -496,6 +496,12 @@
   </si>
   <si>
     <t>Management</t>
+  </si>
+  <si>
+    <t>Miroslav</t>
+  </si>
+  <si>
+    <t>Havelka</t>
   </si>
 </sst>
 </file>
@@ -1042,48 +1048,48 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % – Zvýraznění 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % – Zvýraznění 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % – Zvýraznění 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % – Zvýraznění 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % – Zvýraznění 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % – Zvýraznění 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % – Zvýraznění 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % – Zvýraznění 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % – Zvýraznění 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % – Zvýraznění 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % – Zvýraznění 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % – Zvýraznění 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % – Zvýraznění 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % – Zvýraznění 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % – Zvýraznění 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % – Zvýraznění 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % – Zvýraznění 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % – Zvýraznění 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Celkem" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Kontrolní buňka" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Nadpis 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Nadpis 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Nadpis 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Nadpis 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Název" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Neutrální" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
-    <cellStyle name="Poznámka" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Propojená buňka" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Správně" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Špatně" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Text upozornění" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Vstup" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Výpočet" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Výstup" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Vysvětlující text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Zvýraznění 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Zvýraznění 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Zvýraznění 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Zvýraznění 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Zvýraznění 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Zvýraznění 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1099,7 +1105,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1395,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +1498,7 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(42)&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(10,99)&amp;RANDBETWEEN(10,99)&amp;CHAR(35)&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(10,99)</f>
-        <v>H*T9348#P65</v>
+        <v>M*A5124#K15</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -1530,11 +1536,32 @@
       <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="4">
-        <v>363</v>
-      </c>
+      <c r="P3" s="4"/>
       <c r="Q3" s="5">
         <v>728666999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>_xlfn.CONCAT(E4, " ", F4)</f>
+        <v>Miroslav Havelka</v>
+      </c>
+      <c r="B4" t="str">
+        <f>CONCATENATE(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($E4,"á","a"),"č","c"),"ď","d"),"ě","e"),"é","e"),"í","i"),"ľ","l"),"ň","n"),"ó","o"),"ö","o"),"ř","r"),"š","s"),"ť","t"),"ú","u"),"ů","u"),"ý","y"),"ž","z"),"á","a"),"č","c"),"ď","d"),"ě","e"),"é","e"),"í","i"),"ľ","l"),"ň","n"),"ó","o"),"ö","o"),"ř","r"),"š","s"),"ť","t"),"ú","u"),"ů","u"),"ý","y"),"ž","z")), "_", LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($F4,"á","a"),"č","c"),"ď","d"),"ě","e"),"é","e"),"í","i"),"ľ","l"),"ň","n"),"ó","o"),"ö","o"),"ř","r"),"š","s"),"ť","t"),"ú","u"),"ů","u"),"ý","y"),"ž","z"),"á","a"),"č","c"),"ď","d"),"ě","e"),"é","e"),"í","i"),"ľ","l"),"ň","n"),"ó","o"),"ö","o"),"ř","r"),"š","s"),"ť","t"),"ú","u"),"ů","u"),"ý","y"),"ž","z")), "@mblab.cloud")</f>
+        <v>miroslav_havelka@mblab.cloud</v>
+      </c>
+      <c r="C4" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(42)&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(10,99)&amp;RANDBETWEEN(10,99)&amp;CHAR(35)&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(10,99)</f>
+        <v>F*P3021#J79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>